<commit_message>
quickerSortServer und Excel sheet fertig
</commit_message>
<xml_diff>
--- a/Praktikas/ADS-Praktikum12/src/main/java/Praktikum_12_Code/Laufzeitdiagramm.xlsx
+++ b/Praktikas/ADS-Praktikum12/src/main/java/Praktikum_12_Code/Laufzeitdiagramm.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/spij_zhaw_ch/Documents/Vorlesung/ADS Algorithmen und Datenstrukturen/2020HS/Praktikum/Praktikum 12/A_Aufgabenstellung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucaa/Developer/ADS-Praktikum/Praktikas/ADS-Praktikum12/src/main/java/Praktikum_12_Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{3D298ACD-4096-4991-9068-646D85E00D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8E3A5084-0BFD-4D75-A7F0-3F51EA011DCD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12A8530-69AF-8848-9E76-CCA8F492AC70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{FBA53C49-DF15-4E98-B3C5-5941A6EE6C86}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26600" xr2:uid="{FBA53C49-DF15-4E98-B3C5-5941A6EE6C86}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -70,7 +79,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -88,7 +97,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -150,7 +159,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -274,64 +283,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>102.12</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.11</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.09</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87.99</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>94.88</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88.35</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87.8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>91.96</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.78</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.19</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>93.14</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>95.91</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>92.72</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>98.83</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>96.93</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>96.96</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>105.31</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>102.06</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>101.39</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>104.6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -426,7 +435,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -464,7 +473,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="514769912"/>
@@ -543,7 +552,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -581,7 +590,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="514769584"/>
@@ -622,7 +631,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1231,7 +1240,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1529,13 +1538,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88ABD97-2A93-420F-9FE7-E3359252456A}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B21"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1543,183 +1552,183 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>25</v>
       </c>
       <c r="B2">
-        <v>102.12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+25</f>
         <v>50</v>
       </c>
       <c r="B3">
-        <v>92.11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A21" si="0">A3+25</f>
         <v>75</v>
       </c>
       <c r="B4">
-        <v>90.09</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="B5">
-        <v>87.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
       <c r="B6">
-        <v>94.88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="B7">
-        <v>88.35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
       <c r="B8">
-        <v>87.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="B9">
-        <v>91.96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
       <c r="B10">
-        <v>89.78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
       <c r="B11">
-        <v>92.19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>275</v>
       </c>
       <c r="B12">
-        <v>93.14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B13">
-        <v>95.91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
       <c r="B14">
-        <v>92.72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
       <c r="B15">
-        <v>98.83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>375</v>
       </c>
       <c r="B16">
-        <v>96.93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
       <c r="B17">
-        <v>96.96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>425</v>
       </c>
       <c r="B18">
-        <v>105.31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>450</v>
       </c>
       <c r="B19">
-        <v>102.06</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>475</v>
       </c>
       <c r="B20">
-        <v>101.39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="B21">
-        <v>104.6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>